<commit_message>
feat: Implement Oxygen Scarcity Risk Amplifier and Ventilator Triage Logic
</commit_message>
<xml_diff>
--- a/Patient_Clinical_Data.xlsx
+++ b/Patient_Clinical_Data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R104"/>
+  <dimension ref="A1:R105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6838,10 +6838,8 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>103</t>
-        </is>
+      <c r="A104" t="n">
+        <v>103</v>
       </c>
       <c r="B104" t="n">
         <v>100</v>
@@ -6898,6 +6896,70 @@
         <v>95</v>
       </c>
       <c r="R104" t="n">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>104</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>47</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>80</v>
+      </c>
+      <c r="E105" t="n">
+        <v>120</v>
+      </c>
+      <c r="F105" t="n">
+        <v>80</v>
+      </c>
+      <c r="G105" t="n">
+        <v>98</v>
+      </c>
+      <c r="H105" t="n">
+        <v>37</v>
+      </c>
+      <c r="I105" t="n">
+        <v>16</v>
+      </c>
+      <c r="J105" t="n">
+        <v>120</v>
+      </c>
+      <c r="K105" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="L105" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="n">
+        <v>1</v>
+      </c>
+      <c r="N105" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>Emergency</t>
+        </is>
+      </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>Cardiovascular</t>
+        </is>
+      </c>
+      <c r="Q105" t="n">
+        <v>95</v>
+      </c>
+      <c r="R105" t="n">
         <v>14.5</v>
       </c>
     </row>

</xml_diff>